<commit_message>
code qui ne marche pas (probleme d'input tensorflow)
</commit_message>
<xml_diff>
--- a/Documentation/journal de travail.xlsx
+++ b/Documentation/journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -186,6 +186,18 @@
   </si>
   <si>
     <t>Implémentation d'un système de création de dataset avec enregistrement des labels dans un fichier csv</t>
+  </si>
+  <si>
+    <t>Modification de l'interface</t>
+  </si>
+  <si>
+    <t>L'interface donne maintenant (en temps réel) la largeur et la hauteur de la selectionbox, et les labels deviennent verts quand les proportions de l'échantillon sélectionné permettent d'enregistrer celui-ci sans (trop) le déformer. J'ai aussi commencé à développer un système permettant à l'utilisateur de lire les caractères, et enregistrer les valeurs lues dans un fichier csv, permettant ainsi de faire des paires échantillon/label, qui serviront ensuite à l'entraînement de réseau.</t>
+  </si>
+  <si>
+    <t>Développement d'un système d'importation de datasets</t>
+  </si>
+  <si>
+    <t>L'application est désormais capable d'importer un dataset composé d'un dossier rempli d'images, et d'un fichier csv</t>
   </si>
 </sst>
 </file>
@@ -794,8 +806,8 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,18 +1351,36 @@
       <c r="D41" s="8"/>
       <c r="E41" s="19"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
+    <row r="42" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
+        <v>43256</v>
+      </c>
+      <c r="B42" s="12">
+        <v>6</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>43257</v>
+      </c>
+      <c r="B43" s="5">
+        <v>2</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="E43" s="6"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>